<commit_message>
versión enviada a SCyT
</commit_message>
<xml_diff>
--- a/2023/Formulario-Memoria_VF-2023.xlsx
+++ b/2023/Formulario-Memoria_VF-2023.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="271">
   <si>
     <t xml:space="preserve">FORMULARIO PARA LA CONFECCIÓN DE MEMORIAS DE CENTROS Y GRUPOS</t>
   </si>
@@ -868,18 +868,6 @@
     <t xml:space="preserve">10.4.- Contrato de Asistencia Técnica o Consultoría</t>
   </si>
   <si>
-    <t xml:space="preserve">Optimización de energía de aireación en silos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heebda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heedba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se realiza una propuesta de optimización del sistema de aireación de granos en silos de almacenamiento, con el propósito de ahorrar energía eléctrica en estos sistemas.</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.5.- Servicios técnicos y/o ensayos de laboratorio: breve descripción</t>
   </si>
   <si>
@@ -932,21 +920,52 @@
   </si>
   <si>
     <t xml:space="preserve">Las actividades planificadas para el año 2023 son: 
+ Iniciar los proyectos PID UTN MATCLP10087C, “Estudio de propiedades dinámicas y estructurales
+de materiales granulares” (1/4/2024 – 31/3/2027) y ENECLP0010122 (1/4/2024 – 31/3/2027), “Inci-
+dencia de la viscosidad del fluido en el transporte del agente de sostén dentro de una fractura de
+yacimiento no convencional”. En el primer caso se analizará la dinámica de descarga de un silo en
+dos dimensiones sometido a vibraciones bi-armónicas por medio de simulaciones computacionales,
+mientras que en el segundo se caracterizarán diferentes propiedades reológicas de fluidos y sus efec-
+tos en el transporte de material granular dentro de una celda de ensayo de fracturas.
  Continuar con el desarrollo de los proyectos en ejecución:
- - PID MAUTILP0007746TC: Caracterizar las cadenas de fuerzas en granos con forma pentagonal en el fenómeno de stick-slip  en una geometría Couette, y comparar con los resultados obtenidos para discos. Estudiar la formación de agregados magnéticos en sistemas confinados en dos dimensiones, mediante simulaciones computacionales y experimentos.
- - PICT-2020-SERIEA-I-GRF-00457: Se realizarán mediciones de calibración con el prototipo desarrollado en medios canónicos (respuesta dieléctrica conocida) y se contrastarán con resultados analíticos y de simulación. Asimismo, se continuará con el desarrollo del software  de métodos directo e inverso.
- - PICT-2020-SERIEA-I-GRF-02611: Se avanzará en la caracterización del estado tensional de silos con paredes lisas y rugosas, tanto experimentalmente como a través de simulaciones computacionales.
- - PIP 11220200100717CO: Se desarrollarán experimentos para el análisis del estado tensional y estructural de descarga forzada de silos con diferentes configuraciones de llenado. Se intentará modelar computacionalmente estas configuraciones para obtener resultados numéricos complementarios. 
- Redactar y publicar al menos seis trabajos en revistas internacionales con referato, producto de las investigaciones en las líneas de trabajo actualmente en desarrollo en el GMG. 
- Participar en al menos tres congresos nacionales y uno internacional. 
- Progresar en el desarrollo de los planes de tesis doctorales en curso. 
- Avanzar en la consolidación de las líneas de trabajo de los investigadores jóvenes. 
- Incorporar becarios estudiantes y graduados. 
- Continuar y consolidar las colaboraciones existentes con la empresa Y-TEC, el New Jersey Institute of Technology (USA), la Universidad de Navarra y el Instituto de Química Física Rocasolano (España). Mantener las colaboraciones activas con el Instituto de Física de Liquidos y Sistemas Biológicos, la Universidad Nacional de La Pampa, la Universidad de Buenos Aires y el Centro Atómico Bariloche. 
- Desarrollar el proyecto FITBA A64 en colaboración con la fábrica de implementos agrícolas Heedba. 
- Dictar cursos de grado y posgrado. 
- Incorporar a becarios del GMG a la Carrera del Docente Investigador UTN. 
- Participar en las actividades que proponga la Secretaría de Ciencia y Tecnología de la Facultad Regional La Plata.</t>
+• PID: MAUTNLP0009875: Se continuará con las mediciones experimentales de presión en la
+base de los silos prototipo, y se construirán dos nuevos modelos complementarios para realizar
+experimentos con paredes de diferentes rugosidades.
+• PID: MAECLP0009851TC: Continuación de trabajos con modelos de torso completo, ahora en
+lugar de evaluar ablaciones auriculares comenzaremos a trabajar en ablaciones pericárdicas en
+ventrículo. Adicionalmente, continuaremos con la simulación de la biomecánica de columna
+con discoplastía y comenzaremos con una línea de evaluación experimental y computacional
+de PMMA en modelos de vértebras con discoplastía.
+• PICT-2020-SERIEA-I-GRF-00457: Se realizarán mediciones de calibración con el prototipo desa-
+rrollado en medios canónicos (respuesta dieléctrica conocida) y se contrastarán con resultados
+analíticos y de simulación. Asimismo, se continuará con el desarrollo del software de métodos
+directo e inverso.
+• PICT-2020-SERIEA-I-GRF-02611: Continuaremos con los trabajos de simulación sobre silos con
+paredes de diferentes rugosidades y medidas de presión tanto en simulaciones como en experi-
+mentos. La alumna de Lic. en Física presentará su trabajo final sobre los experimentos y simu-
+laciones llevadas a cabo sobre carga y descarga de silos con diferentes protocolos de llenado.
+• PICT-2021-I-A-00294: Se finalizará el desarrollo del código de simulación de un amortiguador
+granular en dos dimensiones, cuya optimización geométrica se realizará por medio de un algo-
+ritmo genético. Se avanzará en el estudio experimental del efecto de la inclusión de obstáculos
+en un amortiguador granular.
+• PIP 11220200100717CO: Se continuará trabajando con modelos teóricos sobre caudal de partí-
+culas por orificios con y sin forzado. Se estudiarán experimentos sobre optimización de flujo
+de partículas mono y polidispersas.
+• FITBA A64: Se finalizará el proyecto realizando las mediciones del sistema optimizado en silos
+reales de la fábrica Heedba, en la ciudad de 9 de Julio. Redactar y publicar al menos siete trabajos en revistas internacionales con referato, producto de las
+investigaciones en las líneas de trabajo actualmente en desarrollo en el GMG.
+ Participar en al menos tres congresos nacionales y uno internacional.
+ Progresar en el desarrollo de los planes de tesis doctorales en curso.
+ Avanzar en la consolidación de las líneas de trabajo de los investigadores jóvenes.
+ Incorporar becarios estudiantes y graduados.
+ Continuar y consolidar las colaboraciones existentes con la empresa Y-TEC, el New Jersey Institute
+of Technology (USA), la Universidad de Navarra y el Instituto de Química Física Rocasolano (España).
+Mantener las colaboraciones activas con el Instituto de Física de Líquidos y Sistemas Biológicos, la
+Universidad Nacional de La Pampa, la Universidad de Buenos Aires y el Centro Atómico Bariloche.
+ Dictar cursos de grado y posgrado.
+ Incorporar a becarios del GMG a la Carrera del Docente Investigador UTN.
+ Participar en las actividades que proponga la Secretaría de Ciencia y Tecnología de la Facultad Re-
+gional La Plata.</t>
   </si>
 </sst>
 </file>
@@ -957,7 +976,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -987,12 +1006,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1119,7 +1132,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1188,10 +1201,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1230,10 +1239,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1449,8 +1454,8 @@
   </sheetPr>
   <dimension ref="A1:J495"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A440" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I462" activeCellId="0" sqref="I462"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A468" activeCellId="0" sqref="A468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2104,8 +2109,6 @@
       <c r="A44" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -4478,7 +4481,7 @@
       <c r="I214" s="3"/>
       <c r="J214" s="3"/>
     </row>
-    <row r="215" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="7"/>
       <c r="B215" s="7"/>
       <c r="C215" s="7"/>
@@ -4490,7 +4493,7 @@
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
     </row>
-    <row r="216" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="216" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="12" t="s">
         <v>109</v>
       </c>
@@ -4504,7 +4507,7 @@
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
     </row>
-    <row r="217" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="217" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="12" t="s">
         <v>110</v>
       </c>
@@ -4518,7 +4521,7 @@
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
     </row>
-    <row r="218" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="218" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="12" t="s">
         <v>111</v>
       </c>
@@ -4532,7 +4535,7 @@
       <c r="I218" s="3"/>
       <c r="J218" s="3"/>
     </row>
-    <row r="219" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="219" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="12" t="s">
         <v>112</v>
       </c>
@@ -4546,7 +4549,7 @@
       <c r="I219" s="3"/>
       <c r="J219" s="3"/>
     </row>
-    <row r="220" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="12"/>
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
@@ -4558,7 +4561,7 @@
       <c r="I220" s="3"/>
       <c r="J220" s="3"/>
     </row>
-    <row r="221" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="4"/>
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
@@ -4570,7 +4573,7 @@
       <c r="I221" s="3"/>
       <c r="J221" s="3"/>
     </row>
-    <row r="222" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="222" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="12" t="s">
         <v>113</v>
       </c>
@@ -4584,7 +4587,7 @@
       <c r="I222" s="3"/>
       <c r="J222" s="3"/>
     </row>
-    <row r="223" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="12"/>
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
@@ -4596,7 +4599,7 @@
       <c r="I223" s="3"/>
       <c r="J223" s="3"/>
     </row>
-    <row r="224" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="12"/>
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
@@ -4608,7 +4611,7 @@
       <c r="I224" s="3"/>
       <c r="J224" s="3"/>
     </row>
-    <row r="225" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="12"/>
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
@@ -4620,7 +4623,7 @@
       <c r="I225" s="3"/>
       <c r="J225" s="3"/>
     </row>
-    <row r="226" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="12"/>
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
@@ -4632,7 +4635,7 @@
       <c r="I226" s="3"/>
       <c r="J226" s="3"/>
     </row>
-    <row r="227" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="12"/>
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
@@ -4644,7 +4647,7 @@
       <c r="I227" s="3"/>
       <c r="J227" s="3"/>
     </row>
-    <row r="228" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="4"/>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
@@ -4656,7 +4659,7 @@
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
     </row>
-    <row r="229" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="229" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="12" t="s">
         <v>114</v>
       </c>
@@ -4670,7 +4673,7 @@
       <c r="I229" s="3"/>
       <c r="J229" s="3"/>
     </row>
-    <row r="230" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="12"/>
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
@@ -4682,7 +4685,7 @@
       <c r="I230" s="3"/>
       <c r="J230" s="3"/>
     </row>
-    <row r="231" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="12"/>
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
@@ -4694,7 +4697,7 @@
       <c r="I231" s="3"/>
       <c r="J231" s="3"/>
     </row>
-    <row r="232" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="12"/>
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
@@ -4706,7 +4709,7 @@
       <c r="I232" s="3"/>
       <c r="J232" s="3"/>
     </row>
-    <row r="233" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="12"/>
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
@@ -4718,7 +4721,7 @@
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
     </row>
-    <row r="234" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="4"/>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
@@ -4730,7 +4733,7 @@
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
     </row>
-    <row r="235" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="235" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="12" t="s">
         <v>115</v>
       </c>
@@ -4744,7 +4747,7 @@
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
     </row>
-    <row r="236" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="12"/>
       <c r="B236" s="12"/>
       <c r="C236" s="12"/>
@@ -4756,7 +4759,7 @@
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
     </row>
-    <row r="237" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="12"/>
       <c r="B237" s="12"/>
       <c r="C237" s="12"/>
@@ -4768,7 +4771,7 @@
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
     </row>
-    <row r="238" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="12"/>
       <c r="B238" s="12"/>
       <c r="C238" s="12"/>
@@ -4780,7 +4783,7 @@
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
     </row>
-    <row r="239" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="4"/>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
@@ -4792,7 +4795,7 @@
       <c r="I239" s="3"/>
       <c r="J239" s="3"/>
     </row>
-    <row r="240" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="240" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
         <v>116</v>
       </c>
@@ -4806,7 +4809,7 @@
       <c r="I240" s="3"/>
       <c r="J240" s="3"/>
     </row>
-    <row r="241" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="12"/>
       <c r="B241" s="12"/>
       <c r="C241" s="12"/>
@@ -4818,7 +4821,7 @@
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
     </row>
-    <row r="242" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="12"/>
       <c r="B242" s="12"/>
       <c r="C242" s="12"/>
@@ -4830,7 +4833,7 @@
       <c r="I242" s="3"/>
       <c r="J242" s="3"/>
     </row>
-    <row r="243" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="243" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
         <v>89</v>
       </c>
@@ -4844,7 +4847,7 @@
       <c r="I243" s="3"/>
       <c r="J243" s="3"/>
     </row>
-    <row r="244" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="244" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
         <v>117</v>
       </c>
@@ -4858,7 +4861,7 @@
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
     </row>
-    <row r="245" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="245" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
         <v>118</v>
       </c>
@@ -4872,7 +4875,7 @@
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
     </row>
-    <row r="246" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="246" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
         <v>119</v>
       </c>
@@ -4886,7 +4889,7 @@
       <c r="I246" s="3"/>
       <c r="J246" s="3"/>
     </row>
-    <row r="247" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="12"/>
       <c r="B247" s="12"/>
       <c r="C247" s="12"/>
@@ -4898,7 +4901,7 @@
       <c r="I247" s="3"/>
       <c r="J247" s="3"/>
     </row>
-    <row r="248" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="4"/>
       <c r="B248" s="4"/>
       <c r="C248" s="4"/>
@@ -4910,7 +4913,7 @@
       <c r="I248" s="3"/>
       <c r="J248" s="3"/>
     </row>
-    <row r="249" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="249" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
         <v>120</v>
       </c>
@@ -4924,7 +4927,7 @@
       <c r="I249" s="3"/>
       <c r="J249" s="3"/>
     </row>
-    <row r="250" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="12"/>
       <c r="B250" s="12"/>
       <c r="C250" s="12"/>
@@ -4936,7 +4939,7 @@
       <c r="I250" s="3"/>
       <c r="J250" s="3"/>
     </row>
-    <row r="251" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="12"/>
       <c r="B251" s="12"/>
       <c r="C251" s="12"/>
@@ -4948,7 +4951,7 @@
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
     </row>
-    <row r="252" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="12"/>
       <c r="B252" s="12"/>
       <c r="C252" s="12"/>
@@ -4960,7 +4963,7 @@
       <c r="I252" s="3"/>
       <c r="J252" s="3"/>
     </row>
-    <row r="253" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="12"/>
       <c r="B253" s="12"/>
       <c r="C253" s="12"/>
@@ -4972,7 +4975,7 @@
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
     </row>
-    <row r="254" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="12"/>
       <c r="B254" s="12"/>
       <c r="C254" s="12"/>
@@ -4984,7 +4987,7 @@
       <c r="I254" s="3"/>
       <c r="J254" s="3"/>
     </row>
-    <row r="255" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="4"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4"/>
@@ -4996,7 +4999,7 @@
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
     </row>
-    <row r="256" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="256" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
         <v>121</v>
       </c>
@@ -5010,7 +5013,7 @@
       <c r="I256" s="3"/>
       <c r="J256" s="3"/>
     </row>
-    <row r="257" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="12"/>
       <c r="B257" s="12"/>
       <c r="C257" s="12"/>
@@ -5022,7 +5025,7 @@
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
     </row>
-    <row r="258" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="12"/>
       <c r="B258" s="12"/>
       <c r="C258" s="12"/>
@@ -5034,7 +5037,7 @@
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
     </row>
-    <row r="259" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="12"/>
       <c r="B259" s="12"/>
       <c r="C259" s="12"/>
@@ -5046,7 +5049,7 @@
       <c r="I259" s="3"/>
       <c r="J259" s="3"/>
     </row>
-    <row r="260" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="12"/>
       <c r="B260" s="12"/>
       <c r="C260" s="12"/>
@@ -5058,7 +5061,7 @@
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
     </row>
-    <row r="261" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="4"/>
       <c r="B261" s="4"/>
       <c r="C261" s="4"/>
@@ -5070,7 +5073,7 @@
       <c r="I261" s="3"/>
       <c r="J261" s="3"/>
     </row>
-    <row r="262" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="262" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
         <v>115</v>
       </c>
@@ -5084,7 +5087,7 @@
       <c r="I262" s="3"/>
       <c r="J262" s="3"/>
     </row>
-    <row r="263" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="12"/>
       <c r="B263" s="12"/>
       <c r="C263" s="12"/>
@@ -5096,7 +5099,7 @@
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
     </row>
-    <row r="264" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="12"/>
       <c r="B264" s="12"/>
       <c r="C264" s="12"/>
@@ -5108,7 +5111,7 @@
       <c r="I264" s="3"/>
       <c r="J264" s="3"/>
     </row>
-    <row r="265" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="12"/>
       <c r="B265" s="12"/>
       <c r="C265" s="12"/>
@@ -5120,7 +5123,7 @@
       <c r="I265" s="3"/>
       <c r="J265" s="3"/>
     </row>
-    <row r="266" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="4"/>
       <c r="B266" s="4"/>
       <c r="C266" s="4"/>
@@ -5132,7 +5135,7 @@
       <c r="I266" s="3"/>
       <c r="J266" s="3"/>
     </row>
-    <row r="267" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="267" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
         <v>102</v>
       </c>
@@ -5146,7 +5149,7 @@
       <c r="I267" s="3"/>
       <c r="J267" s="3"/>
     </row>
-    <row r="268" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="12"/>
       <c r="B268" s="12"/>
       <c r="C268" s="12"/>
@@ -5158,7 +5161,7 @@
       <c r="I268" s="3"/>
       <c r="J268" s="3"/>
     </row>
-    <row r="269" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="12"/>
       <c r="B269" s="12"/>
       <c r="C269" s="12"/>
@@ -5170,7 +5173,7 @@
       <c r="I269" s="3"/>
       <c r="J269" s="3"/>
     </row>
-    <row r="270" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="270" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
         <v>95</v>
       </c>
@@ -5184,7 +5187,7 @@
       <c r="I270" s="3"/>
       <c r="J270" s="3"/>
     </row>
-    <row r="271" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="271" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
         <v>122</v>
       </c>
@@ -5198,7 +5201,7 @@
       <c r="I271" s="3"/>
       <c r="J271" s="3"/>
     </row>
-    <row r="272" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="272" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
         <v>118</v>
       </c>
@@ -5212,7 +5215,7 @@
       <c r="I272" s="3"/>
       <c r="J272" s="3"/>
     </row>
-    <row r="273" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="273" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="12" t="s">
         <v>123</v>
       </c>
@@ -5226,7 +5229,7 @@
       <c r="I273" s="3"/>
       <c r="J273" s="3"/>
     </row>
-    <row r="274" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="12"/>
       <c r="B274" s="12"/>
       <c r="C274" s="12"/>
@@ -5238,7 +5241,7 @@
       <c r="I274" s="3"/>
       <c r="J274" s="3"/>
     </row>
-    <row r="275" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="4"/>
       <c r="B275" s="4"/>
       <c r="C275" s="4"/>
@@ -5250,7 +5253,7 @@
       <c r="I275" s="3"/>
       <c r="J275" s="3"/>
     </row>
-    <row r="276" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="276" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
         <v>124</v>
       </c>
@@ -5264,7 +5267,7 @@
       <c r="I276" s="3"/>
       <c r="J276" s="3"/>
     </row>
-    <row r="277" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="12"/>
       <c r="B277" s="12"/>
       <c r="C277" s="12"/>
@@ -5276,7 +5279,7 @@
       <c r="I277" s="3"/>
       <c r="J277" s="3"/>
     </row>
-    <row r="278" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="12"/>
       <c r="B278" s="12"/>
       <c r="C278" s="12"/>
@@ -5288,7 +5291,7 @@
       <c r="I278" s="3"/>
       <c r="J278" s="3"/>
     </row>
-    <row r="279" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="12"/>
       <c r="B279" s="12"/>
       <c r="C279" s="12"/>
@@ -5300,7 +5303,7 @@
       <c r="I279" s="3"/>
       <c r="J279" s="3"/>
     </row>
-    <row r="280" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="12"/>
       <c r="B280" s="12"/>
       <c r="C280" s="12"/>
@@ -5312,7 +5315,7 @@
       <c r="I280" s="3"/>
       <c r="J280" s="3"/>
     </row>
-    <row r="281" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="12"/>
       <c r="B281" s="12"/>
       <c r="C281" s="12"/>
@@ -5324,7 +5327,7 @@
       <c r="I281" s="3"/>
       <c r="J281" s="3"/>
     </row>
-    <row r="282" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="4"/>
       <c r="B282" s="4"/>
       <c r="C282" s="4"/>
@@ -5336,7 +5339,7 @@
       <c r="I282" s="3"/>
       <c r="J282" s="3"/>
     </row>
-    <row r="283" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="283" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
         <v>125</v>
       </c>
@@ -5350,7 +5353,7 @@
       <c r="I283" s="3"/>
       <c r="J283" s="3"/>
     </row>
-    <row r="284" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="12"/>
       <c r="B284" s="12"/>
       <c r="C284" s="12"/>
@@ -5362,7 +5365,7 @@
       <c r="I284" s="3"/>
       <c r="J284" s="3"/>
     </row>
-    <row r="285" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="12"/>
       <c r="B285" s="12"/>
       <c r="C285" s="12"/>
@@ -5374,7 +5377,7 @@
       <c r="I285" s="3"/>
       <c r="J285" s="3"/>
     </row>
-    <row r="286" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="12"/>
       <c r="B286" s="12"/>
       <c r="C286" s="12"/>
@@ -5386,7 +5389,7 @@
       <c r="I286" s="3"/>
       <c r="J286" s="3"/>
     </row>
-    <row r="287" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="12"/>
       <c r="B287" s="12"/>
       <c r="C287" s="12"/>
@@ -5398,7 +5401,7 @@
       <c r="I287" s="3"/>
       <c r="J287" s="3"/>
     </row>
-    <row r="288" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="4"/>
       <c r="B288" s="4"/>
       <c r="C288" s="4"/>
@@ -5410,7 +5413,7 @@
       <c r="I288" s="3"/>
       <c r="J288" s="3"/>
     </row>
-    <row r="289" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="289" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
         <v>115</v>
       </c>
@@ -5424,7 +5427,7 @@
       <c r="I289" s="3"/>
       <c r="J289" s="3"/>
     </row>
-    <row r="290" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="12"/>
       <c r="B290" s="12"/>
       <c r="C290" s="12"/>
@@ -5436,7 +5439,7 @@
       <c r="I290" s="3"/>
       <c r="J290" s="3"/>
     </row>
-    <row r="291" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12"/>
       <c r="B291" s="12"/>
       <c r="C291" s="12"/>
@@ -5448,7 +5451,7 @@
       <c r="I291" s="3"/>
       <c r="J291" s="3"/>
     </row>
-    <row r="292" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="12"/>
       <c r="B292" s="12"/>
       <c r="C292" s="12"/>
@@ -5460,7 +5463,7 @@
       <c r="I292" s="3"/>
       <c r="J292" s="3"/>
     </row>
-    <row r="293" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="4"/>
       <c r="B293" s="4"/>
       <c r="C293" s="4"/>
@@ -5472,7 +5475,7 @@
       <c r="I293" s="3"/>
       <c r="J293" s="3"/>
     </row>
-    <row r="294" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="294" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="12" t="s">
         <v>102</v>
       </c>
@@ -5486,7 +5489,7 @@
       <c r="I294" s="3"/>
       <c r="J294" s="3"/>
     </row>
-    <row r="295" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="12"/>
       <c r="B295" s="12"/>
       <c r="C295" s="12"/>
@@ -5498,7 +5501,7 @@
       <c r="I295" s="3"/>
       <c r="J295" s="3"/>
     </row>
-    <row r="296" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="12"/>
       <c r="B296" s="12"/>
       <c r="C296" s="12"/>
@@ -5510,7 +5513,7 @@
       <c r="I296" s="3"/>
       <c r="J296" s="3"/>
     </row>
-    <row r="297" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="297" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
         <v>126</v>
       </c>
@@ -5524,7 +5527,7 @@
       <c r="I297" s="3"/>
       <c r="J297" s="3"/>
     </row>
-    <row r="298" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="298" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
         <v>127</v>
       </c>
@@ -5538,7 +5541,7 @@
       <c r="I298" s="3"/>
       <c r="J298" s="3"/>
     </row>
-    <row r="299" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="299" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
         <v>128</v>
       </c>
@@ -5552,7 +5555,7 @@
       <c r="I299" s="3"/>
       <c r="J299" s="3"/>
     </row>
-    <row r="300" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="300" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
         <v>129</v>
       </c>
@@ -5566,7 +5569,7 @@
       <c r="I300" s="3"/>
       <c r="J300" s="3"/>
     </row>
-    <row r="301" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="12"/>
       <c r="B301" s="12"/>
       <c r="C301" s="12"/>
@@ -5578,7 +5581,7 @@
       <c r="I301" s="3"/>
       <c r="J301" s="3"/>
     </row>
-    <row r="302" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="4"/>
       <c r="B302" s="4"/>
       <c r="C302" s="4"/>
@@ -5590,7 +5593,7 @@
       <c r="I302" s="3"/>
       <c r="J302" s="3"/>
     </row>
-    <row r="303" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="303" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
         <v>130</v>
       </c>
@@ -5604,7 +5607,7 @@
       <c r="I303" s="3"/>
       <c r="J303" s="3"/>
     </row>
-    <row r="304" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
       <c r="C304" s="12"/>
@@ -5616,7 +5619,7 @@
       <c r="I304" s="3"/>
       <c r="J304" s="3"/>
     </row>
-    <row r="305" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="12"/>
       <c r="B305" s="12"/>
       <c r="C305" s="12"/>
@@ -5628,7 +5631,7 @@
       <c r="I305" s="3"/>
       <c r="J305" s="3"/>
     </row>
-    <row r="306" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="12"/>
       <c r="B306" s="12"/>
       <c r="C306" s="12"/>
@@ -5640,7 +5643,7 @@
       <c r="I306" s="3"/>
       <c r="J306" s="3"/>
     </row>
-    <row r="307" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="12"/>
       <c r="B307" s="12"/>
       <c r="C307" s="12"/>
@@ -5652,7 +5655,7 @@
       <c r="I307" s="3"/>
       <c r="J307" s="3"/>
     </row>
-    <row r="308" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12"/>
       <c r="B308" s="12"/>
       <c r="C308" s="12"/>
@@ -5664,7 +5667,7 @@
       <c r="I308" s="3"/>
       <c r="J308" s="3"/>
     </row>
-    <row r="309" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="4"/>
       <c r="B309" s="4"/>
       <c r="C309" s="4"/>
@@ -5676,7 +5679,7 @@
       <c r="I309" s="3"/>
       <c r="J309" s="3"/>
     </row>
-    <row r="310" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="310" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
         <v>131</v>
       </c>
@@ -5690,7 +5693,7 @@
       <c r="I310" s="3"/>
       <c r="J310" s="3"/>
     </row>
-    <row r="311" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="12"/>
       <c r="B311" s="12"/>
       <c r="C311" s="12"/>
@@ -5702,7 +5705,7 @@
       <c r="I311" s="3"/>
       <c r="J311" s="3"/>
     </row>
-    <row r="312" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="12"/>
       <c r="B312" s="12"/>
       <c r="C312" s="12"/>
@@ -5714,7 +5717,7 @@
       <c r="I312" s="3"/>
       <c r="J312" s="3"/>
     </row>
-    <row r="313" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="12"/>
       <c r="B313" s="12"/>
       <c r="C313" s="12"/>
@@ -5726,7 +5729,7 @@
       <c r="I313" s="3"/>
       <c r="J313" s="3"/>
     </row>
-    <row r="314" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="12"/>
       <c r="B314" s="12"/>
       <c r="C314" s="12"/>
@@ -5738,7 +5741,7 @@
       <c r="I314" s="3"/>
       <c r="J314" s="3"/>
     </row>
-    <row r="315" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="4"/>
       <c r="B315" s="4"/>
       <c r="C315" s="4"/>
@@ -5750,7 +5753,7 @@
       <c r="I315" s="3"/>
       <c r="J315" s="3"/>
     </row>
-    <row r="316" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="316" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
         <v>132</v>
       </c>
@@ -5764,7 +5767,7 @@
       <c r="I316" s="3"/>
       <c r="J316" s="3"/>
     </row>
-    <row r="317" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="12"/>
       <c r="B317" s="12"/>
       <c r="C317" s="12"/>
@@ -5776,7 +5779,7 @@
       <c r="I317" s="3"/>
       <c r="J317" s="3"/>
     </row>
-    <row r="318" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="12"/>
       <c r="B318" s="12"/>
       <c r="C318" s="12"/>
@@ -5788,7 +5791,7 @@
       <c r="I318" s="3"/>
       <c r="J318" s="3"/>
     </row>
-    <row r="319" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="12"/>
       <c r="B319" s="12"/>
       <c r="C319" s="12"/>
@@ -5800,7 +5803,7 @@
       <c r="I319" s="3"/>
       <c r="J319" s="3"/>
     </row>
-    <row r="320" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="4"/>
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
@@ -5812,7 +5815,7 @@
       <c r="I320" s="3"/>
       <c r="J320" s="3"/>
     </row>
-    <row r="321" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="321" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
         <v>133</v>
       </c>
@@ -5826,7 +5829,7 @@
       <c r="I321" s="3"/>
       <c r="J321" s="3"/>
     </row>
-    <row r="322" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="12"/>
       <c r="B322" s="12"/>
       <c r="C322" s="12"/>
@@ -5839,14 +5842,14 @@
       <c r="J322" s="3"/>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A323" s="18" t="s">
+      <c r="A323" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B323" s="18"/>
-      <c r="C323" s="18"/>
-      <c r="D323" s="18"/>
-      <c r="E323" s="18"/>
-      <c r="F323" s="18"/>
+      <c r="B323" s="17"/>
+      <c r="C323" s="17"/>
+      <c r="D323" s="17"/>
+      <c r="E323" s="17"/>
+      <c r="F323" s="17"/>
       <c r="G323" s="3"/>
       <c r="H323" s="3"/>
       <c r="I323" s="3"/>
@@ -5979,24 +5982,24 @@
       <c r="J333" s="3"/>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="19"/>
+      <c r="A334" s="18"/>
       <c r="B334" s="3"/>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
       <c r="E334" s="3"/>
-      <c r="F334" s="20"/>
+      <c r="F334" s="19"/>
       <c r="G334" s="3"/>
       <c r="H334" s="3"/>
       <c r="I334" s="3"/>
       <c r="J334" s="3"/>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="21"/>
-      <c r="B335" s="22"/>
-      <c r="C335" s="22"/>
-      <c r="D335" s="22"/>
-      <c r="E335" s="22"/>
-      <c r="F335" s="23"/>
+      <c r="A335" s="20"/>
+      <c r="B335" s="21"/>
+      <c r="C335" s="21"/>
+      <c r="D335" s="21"/>
+      <c r="E335" s="21"/>
+      <c r="F335" s="22"/>
       <c r="G335" s="3"/>
       <c r="H335" s="3"/>
       <c r="I335" s="3"/>
@@ -6163,25 +6166,25 @@
       <c r="J345" s="3"/>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="24" t="s">
+      <c r="A346" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B346" s="24" t="s">
+      <c r="B346" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C346" s="24" t="s">
+      <c r="C346" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D346" s="24" t="s">
+      <c r="D346" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E346" s="24" t="s">
+      <c r="E346" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="F346" s="24" t="s">
+      <c r="F346" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="G346" s="24" t="s">
+      <c r="G346" s="23" t="s">
         <v>75</v>
       </c>
       <c r="H346" s="3"/>
@@ -6280,7 +6283,7 @@
       <c r="I350" s="3"/>
       <c r="J350" s="3"/>
     </row>
-    <row r="351" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="15"/>
       <c r="B351" s="15"/>
       <c r="C351" s="15"/>
@@ -6321,7 +6324,7 @@
       <c r="J353" s="3"/>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="26" t="s">
+      <c r="A354" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B354" s="7" t="s">
@@ -6372,7 +6375,7 @@
       <c r="I355" s="3"/>
       <c r="J355" s="3"/>
     </row>
-    <row r="356" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="7" t="n">
         <v>2</v>
       </c>
@@ -6411,7 +6414,7 @@
       <c r="D357" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E357" s="27" t="n">
+      <c r="E357" s="26" t="n">
         <v>8873585</v>
       </c>
       <c r="F357" s="12" t="s">
@@ -6437,7 +6440,7 @@
       <c r="D358" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E358" s="27" t="n">
+      <c r="E358" s="26" t="n">
         <v>22277390</v>
       </c>
       <c r="F358" s="12" t="s">
@@ -6463,7 +6466,7 @@
       <c r="D359" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E359" s="27" t="n">
+      <c r="E359" s="26" t="n">
         <v>24700045</v>
       </c>
       <c r="F359" s="12" t="s">
@@ -6489,7 +6492,7 @@
       <c r="D360" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="E360" s="27" t="n">
+      <c r="E360" s="26" t="n">
         <v>325910</v>
       </c>
       <c r="F360" s="7" t="s">
@@ -6515,7 +6518,7 @@
       <c r="D361" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="E361" s="27" t="n">
+      <c r="E361" s="26" t="n">
         <v>10995129</v>
       </c>
       <c r="F361" s="7" t="s">
@@ -6538,10 +6541,10 @@
       <c r="C362" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D362" s="28" t="s">
+      <c r="D362" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E362" s="27" t="n">
+      <c r="E362" s="26" t="n">
         <v>14203049</v>
       </c>
       <c r="F362" s="7" t="s">
@@ -6567,7 +6570,7 @@
       <c r="D363" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E363" s="29" t="s">
+      <c r="E363" s="27" t="s">
         <v>211</v>
       </c>
       <c r="F363" s="12" t="s">
@@ -6587,7 +6590,7 @@
       <c r="B364" s="7"/>
       <c r="C364" s="7"/>
       <c r="D364" s="7"/>
-      <c r="E364" s="27"/>
+      <c r="E364" s="26"/>
       <c r="F364" s="7"/>
       <c r="G364" s="7"/>
       <c r="H364" s="3"/>
@@ -6601,7 +6604,7 @@
       <c r="B365" s="7"/>
       <c r="C365" s="7"/>
       <c r="D365" s="7"/>
-      <c r="E365" s="27"/>
+      <c r="E365" s="26"/>
       <c r="F365" s="7"/>
       <c r="G365" s="7"/>
       <c r="H365" s="3"/>
@@ -6921,12 +6924,12 @@
       <c r="J390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="30"/>
-      <c r="B391" s="30"/>
-      <c r="C391" s="30"/>
-      <c r="D391" s="30"/>
-      <c r="E391" s="30"/>
-      <c r="F391" s="30"/>
+      <c r="A391" s="28"/>
+      <c r="B391" s="28"/>
+      <c r="C391" s="28"/>
+      <c r="D391" s="28"/>
+      <c r="E391" s="28"/>
+      <c r="F391" s="28"/>
       <c r="G391" s="3"/>
       <c r="H391" s="3"/>
       <c r="I391" s="3"/>
@@ -6936,11 +6939,11 @@
       <c r="A392" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B392" s="31"/>
-      <c r="C392" s="31"/>
-      <c r="D392" s="31"/>
-      <c r="E392" s="31"/>
-      <c r="F392" s="31"/>
+      <c r="B392" s="29"/>
+      <c r="C392" s="29"/>
+      <c r="D392" s="29"/>
+      <c r="E392" s="29"/>
+      <c r="F392" s="29"/>
       <c r="G392" s="3"/>
       <c r="H392" s="3"/>
       <c r="I392" s="3"/>
@@ -7101,12 +7104,12 @@
       <c r="J400" s="3"/>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="32"/>
-      <c r="B401" s="33"/>
-      <c r="C401" s="33"/>
-      <c r="D401" s="33"/>
-      <c r="E401" s="33"/>
-      <c r="F401" s="33"/>
+      <c r="A401" s="30"/>
+      <c r="B401" s="31"/>
+      <c r="C401" s="31"/>
+      <c r="D401" s="31"/>
+      <c r="E401" s="31"/>
+      <c r="F401" s="31"/>
       <c r="G401" s="3"/>
       <c r="H401" s="3"/>
       <c r="I401" s="3"/>
@@ -7516,29 +7519,15 @@
       <c r="A427" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B427" s="7" t="s">
-        <v>253</v>
-      </c>
+      <c r="B427" s="7"/>
       <c r="C427" s="7"/>
-      <c r="D427" s="7" t="s">
-        <v>254</v>
-      </c>
+      <c r="D427" s="7"/>
       <c r="E427" s="7"/>
-      <c r="F427" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="G427" s="14" t="n">
-        <v>44979</v>
-      </c>
-      <c r="H427" s="14" t="n">
-        <v>45344</v>
-      </c>
-      <c r="I427" s="7" t="n">
-        <v>7850000</v>
-      </c>
-      <c r="J427" s="7" t="s">
-        <v>256</v>
-      </c>
+      <c r="F427" s="7"/>
+      <c r="G427" s="14"/>
+      <c r="H427" s="14"/>
+      <c r="I427" s="7"/>
+      <c r="J427" s="7"/>
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="n">
@@ -7595,18 +7584,18 @@
       <c r="J431" s="3"/>
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="B432" s="34"/>
-      <c r="C432" s="34"/>
-      <c r="D432" s="34"/>
-      <c r="E432" s="34"/>
-      <c r="F432" s="34"/>
-      <c r="G432" s="34"/>
-      <c r="H432" s="34"/>
-      <c r="I432" s="34"/>
-      <c r="J432" s="34"/>
+      <c r="A432" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B432" s="32"/>
+      <c r="C432" s="32"/>
+      <c r="D432" s="32"/>
+      <c r="E432" s="32"/>
+      <c r="F432" s="32"/>
+      <c r="G432" s="32"/>
+      <c r="H432" s="32"/>
+      <c r="I432" s="32"/>
+      <c r="J432" s="32"/>
     </row>
     <row r="433" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
@@ -7718,7 +7707,7 @@
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B440" s="5"/>
       <c r="C440" s="5"/>
@@ -7732,7 +7721,7 @@
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B441" s="5"/>
       <c r="C441" s="5"/>
@@ -7745,30 +7734,30 @@
       <c r="J441" s="3"/>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="35"/>
-      <c r="B442" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="C442" s="35"/>
-      <c r="D442" s="35"/>
-      <c r="E442" s="35"/>
-      <c r="F442" s="35"/>
+      <c r="A442" s="33"/>
+      <c r="B442" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="C442" s="33"/>
+      <c r="D442" s="33"/>
+      <c r="E442" s="33"/>
+      <c r="F442" s="33"/>
       <c r="G442" s="3"/>
       <c r="H442" s="3"/>
       <c r="I442" s="3"/>
       <c r="J442" s="3"/>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A443" s="35"/>
+      <c r="A443" s="33"/>
       <c r="B443" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C443" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D443" s="7"/>
       <c r="E443" s="12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F443" s="12"/>
       <c r="G443" s="3"/>
@@ -7792,9 +7781,13 @@
       <c r="B445" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C445" s="7"/>
+      <c r="C445" s="7" t="n">
+        <v>100000</v>
+      </c>
       <c r="D445" s="7"/>
-      <c r="E445" s="7"/>
+      <c r="E445" s="7" t="n">
+        <v>100000</v>
+      </c>
       <c r="F445" s="7"/>
       <c r="G445" s="3"/>
       <c r="H445" s="3"/>
@@ -7806,11 +7799,15 @@
         <v>2</v>
       </c>
       <c r="B446" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C446" s="7"/>
+        <v>260</v>
+      </c>
+      <c r="C446" s="7" t="n">
+        <v>75000</v>
+      </c>
       <c r="D446" s="7"/>
-      <c r="E446" s="7"/>
+      <c r="E446" s="7" t="n">
+        <v>75000</v>
+      </c>
       <c r="F446" s="7"/>
       <c r="G446" s="3"/>
       <c r="H446" s="3"/>
@@ -7822,11 +7819,15 @@
         <v>3</v>
       </c>
       <c r="B447" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C447" s="7"/>
+        <v>261</v>
+      </c>
+      <c r="C447" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="D447" s="7"/>
-      <c r="E447" s="7"/>
+      <c r="E447" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="F447" s="7"/>
       <c r="G447" s="3"/>
       <c r="H447" s="3"/>
@@ -7838,11 +7839,15 @@
         <v>4</v>
       </c>
       <c r="B448" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C448" s="7"/>
+        <v>262</v>
+      </c>
+      <c r="C448" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="D448" s="7"/>
-      <c r="E448" s="7"/>
+      <c r="E448" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="F448" s="7"/>
       <c r="G448" s="3"/>
       <c r="H448" s="3"/>
@@ -7854,11 +7859,15 @@
         <v>5</v>
       </c>
       <c r="B449" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C449" s="7"/>
+        <v>263</v>
+      </c>
+      <c r="C449" s="7" t="n">
+        <v>286443.9</v>
+      </c>
       <c r="D449" s="7"/>
-      <c r="E449" s="7"/>
+      <c r="E449" s="7" t="n">
+        <v>286443.9</v>
+      </c>
       <c r="F449" s="7"/>
       <c r="G449" s="3"/>
       <c r="H449" s="3"/>
@@ -7870,11 +7879,15 @@
         <v>6</v>
       </c>
       <c r="B450" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C450" s="7"/>
+        <v>264</v>
+      </c>
+      <c r="C450" s="7" t="n">
+        <v>400000</v>
+      </c>
       <c r="D450" s="7"/>
-      <c r="E450" s="7"/>
+      <c r="E450" s="7" t="n">
+        <v>400000</v>
+      </c>
       <c r="F450" s="7"/>
       <c r="G450" s="3"/>
       <c r="H450" s="3"/>
@@ -7886,11 +7899,15 @@
         <v>7</v>
       </c>
       <c r="B451" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C451" s="7"/>
+        <v>265</v>
+      </c>
+      <c r="C451" s="7" t="n">
+        <v>242463.83</v>
+      </c>
       <c r="D451" s="7"/>
-      <c r="E451" s="7"/>
+      <c r="E451" s="7" t="n">
+        <v>242463.83</v>
+      </c>
       <c r="F451" s="7"/>
       <c r="G451" s="3"/>
       <c r="H451" s="3"/>
@@ -7902,11 +7919,15 @@
         <v>8</v>
       </c>
       <c r="B452" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C452" s="7"/>
+        <v>266</v>
+      </c>
+      <c r="C452" s="7" t="n">
+        <v>193966.56</v>
+      </c>
       <c r="D452" s="7"/>
-      <c r="E452" s="7"/>
+      <c r="E452" s="7" t="n">
+        <v>193966.56</v>
+      </c>
       <c r="F452" s="7"/>
       <c r="G452" s="3"/>
       <c r="H452" s="3"/>
@@ -7918,11 +7939,15 @@
         <v>9</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C453" s="7"/>
+        <v>267</v>
+      </c>
+      <c r="C453" s="7" t="n">
+        <v>850000</v>
+      </c>
       <c r="D453" s="7"/>
-      <c r="E453" s="7"/>
+      <c r="E453" s="7" t="n">
+        <v>850000</v>
+      </c>
       <c r="F453" s="7"/>
       <c r="G453" s="3"/>
       <c r="H453" s="3"/>
@@ -7944,7 +7969,7 @@
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7"/>
       <c r="B455" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C455" s="7"/>
       <c r="D455" s="7"/>
@@ -7960,14 +7985,14 @@
         <v>9</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C456" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D456" s="7"/>
       <c r="E456" s="12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F456" s="12"/>
       <c r="G456" s="3"/>
@@ -7982,9 +8007,13 @@
       <c r="B457" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C457" s="7"/>
+      <c r="C457" s="7" t="n">
+        <v>450000</v>
+      </c>
       <c r="D457" s="7"/>
-      <c r="E457" s="7"/>
+      <c r="E457" s="7" t="n">
+        <v>450000</v>
+      </c>
       <c r="F457" s="7"/>
       <c r="G457" s="3"/>
       <c r="H457" s="3"/>
@@ -7996,11 +8025,15 @@
         <v>2</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C458" s="7"/>
+        <v>260</v>
+      </c>
+      <c r="C458" s="7" t="n">
+        <v>75000</v>
+      </c>
       <c r="D458" s="7"/>
-      <c r="E458" s="7"/>
+      <c r="E458" s="7" t="n">
+        <v>75000</v>
+      </c>
       <c r="F458" s="7"/>
       <c r="G458" s="3"/>
       <c r="H458" s="3"/>
@@ -8012,11 +8045,15 @@
         <v>3</v>
       </c>
       <c r="B459" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C459" s="7"/>
+        <v>261</v>
+      </c>
+      <c r="C459" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="D459" s="7"/>
-      <c r="E459" s="7"/>
+      <c r="E459" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="F459" s="7"/>
       <c r="G459" s="3"/>
       <c r="H459" s="3"/>
@@ -8028,11 +8065,15 @@
         <v>4</v>
       </c>
       <c r="B460" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C460" s="7"/>
+        <v>262</v>
+      </c>
+      <c r="C460" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="D460" s="7"/>
-      <c r="E460" s="7"/>
+      <c r="E460" s="7" t="n">
+        <v>270000</v>
+      </c>
       <c r="F460" s="7"/>
       <c r="G460" s="3"/>
       <c r="H460" s="3"/>
@@ -8044,11 +8085,15 @@
         <v>5</v>
       </c>
       <c r="B461" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C461" s="7"/>
+        <v>263</v>
+      </c>
+      <c r="C461" s="7" t="n">
+        <v>64257.56</v>
+      </c>
       <c r="D461" s="7"/>
-      <c r="E461" s="7"/>
+      <c r="E461" s="7" t="n">
+        <v>64257.56</v>
+      </c>
       <c r="F461" s="7"/>
       <c r="G461" s="3"/>
       <c r="H461" s="3"/>
@@ -8060,11 +8105,15 @@
         <v>6</v>
       </c>
       <c r="B462" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C462" s="7"/>
+        <v>264</v>
+      </c>
+      <c r="C462" s="7" t="n">
+        <v>800000</v>
+      </c>
       <c r="D462" s="7"/>
-      <c r="E462" s="7"/>
+      <c r="E462" s="7" t="n">
+        <v>800000</v>
+      </c>
       <c r="F462" s="7"/>
       <c r="G462" s="3"/>
       <c r="H462" s="3"/>
@@ -8076,11 +8125,15 @@
         <v>7</v>
       </c>
       <c r="B463" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C463" s="7"/>
+        <v>265</v>
+      </c>
+      <c r="C463" s="7" t="n">
+        <v>458135.8</v>
+      </c>
       <c r="D463" s="7"/>
-      <c r="E463" s="7"/>
+      <c r="E463" s="7" t="n">
+        <v>458135.8</v>
+      </c>
       <c r="F463" s="7"/>
       <c r="G463" s="3"/>
       <c r="H463" s="3"/>
@@ -8092,11 +8145,15 @@
         <v>8</v>
       </c>
       <c r="B464" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C464" s="7"/>
+        <v>266</v>
+      </c>
+      <c r="C464" s="7" t="n">
+        <v>316033.44</v>
+      </c>
       <c r="D464" s="7"/>
-      <c r="E464" s="7"/>
+      <c r="E464" s="7" t="n">
+        <v>126598</v>
+      </c>
       <c r="F464" s="7"/>
       <c r="G464" s="3"/>
       <c r="H464" s="3"/>
@@ -8108,11 +8165,15 @@
         <v>9</v>
       </c>
       <c r="B465" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C465" s="3"/>
+        <v>267</v>
+      </c>
+      <c r="C465" s="3" t="n">
+        <v>7000000</v>
+      </c>
       <c r="D465" s="3"/>
-      <c r="E465" s="3"/>
+      <c r="E465" s="3" t="n">
+        <v>7000000</v>
+      </c>
       <c r="F465" s="3"/>
       <c r="G465" s="3"/>
       <c r="H465" s="3"/>
@@ -8133,7 +8194,7 @@
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
@@ -8147,7 +8208,7 @@
     </row>
     <row r="468" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A468" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B468" s="8"/>
       <c r="C468" s="8"/>
@@ -8215,7 +8276,6 @@
       <c r="E473" s="8"/>
       <c r="F473" s="8"/>
     </row>
-    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8238,7 +8298,7 @@
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="280">
+  <mergeCells count="292">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
@@ -8495,12 +8555,18 @@
     <mergeCell ref="E446:F446"/>
     <mergeCell ref="C447:D447"/>
     <mergeCell ref="E447:F447"/>
+    <mergeCell ref="C448:D448"/>
+    <mergeCell ref="E448:F448"/>
     <mergeCell ref="C449:D449"/>
     <mergeCell ref="E449:F449"/>
     <mergeCell ref="C450:D450"/>
     <mergeCell ref="E450:F450"/>
+    <mergeCell ref="C451:D451"/>
+    <mergeCell ref="E451:F451"/>
     <mergeCell ref="C452:D452"/>
     <mergeCell ref="E452:F452"/>
+    <mergeCell ref="C453:D453"/>
+    <mergeCell ref="E453:F453"/>
     <mergeCell ref="A454:F454"/>
     <mergeCell ref="B455:F455"/>
     <mergeCell ref="C456:D456"/>
@@ -8517,6 +8583,12 @@
     <mergeCell ref="E461:F461"/>
     <mergeCell ref="C462:D462"/>
     <mergeCell ref="E462:F462"/>
+    <mergeCell ref="C463:D463"/>
+    <mergeCell ref="E463:F463"/>
+    <mergeCell ref="C464:D464"/>
+    <mergeCell ref="E464:F464"/>
+    <mergeCell ref="C465:D465"/>
+    <mergeCell ref="E465:F465"/>
     <mergeCell ref="A467:F467"/>
     <mergeCell ref="A468:F473"/>
   </mergeCells>

</xml_diff>